<commit_message>
Modification about Preference and Creator/Checker
</commit_message>
<xml_diff>
--- a/org.but4reuse.adapters.eclipse/src/resources/TestingPlan.xlsx
+++ b/org.but4reuse.adapters.eclipse/src/resources/TestingPlan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Automotive</t>
   </si>
@@ -41,9 +41,6 @@
     <t>RCP</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
     <t>Reporting</t>
   </si>
   <si>
@@ -56,7 +53,43 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>All (12)</t>
+    <t>Java_Scout</t>
+  </si>
+  <si>
+    <t>JEE_RCP</t>
+  </si>
+  <si>
+    <t>Parallel_CPP</t>
+  </si>
+  <si>
+    <t>Standard_Modeling</t>
+  </si>
+  <si>
+    <t>Automotive_DSL_JEE_Parallel_Reporting</t>
+  </si>
+  <si>
+    <t>CPP_Java_Modeling_RCP_Scout</t>
+  </si>
+  <si>
+    <t>Testing_Scout_Standard_Parallel_CPP</t>
+  </si>
+  <si>
+    <t>Java_JEE_Automotive_Modeling_Testing</t>
+  </si>
+  <si>
+    <t>AllWithoutRCP_Scout</t>
+  </si>
+  <si>
+    <t>AllWithoutJava_JEE</t>
+  </si>
+  <si>
+    <t>AllWithoutStandard_DSL</t>
+  </si>
+  <si>
+    <t>AllWithoutTesting_Reporting</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
   <si>
     <t>Percentage use in input</t>
@@ -65,7 +98,7 @@
     <t>Eclipse use in input</t>
   </si>
   <si>
-    <t>Variant executable ? (V for True, X for false) </t>
+    <t>Executable variant ? (V for true, X for false)</t>
   </si>
 </sst>
 </file>
@@ -75,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -111,9 +144,17 @@
       <color rgb="FF0000FF"/>
       <name val="Cambria"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
@@ -123,7 +164,6 @@
       <color rgb="FF0000FF"/>
       <name val="Cambria"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -156,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="34">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -440,6 +480,51 @@
         <color rgb="FF666666"/>
       </top>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="dotted">
+        <color rgb="FF666666"/>
+      </right>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dotted">
+        <color rgb="FF666666"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF666666"/>
+      </right>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dotted">
+        <color rgb="FF666666"/>
+      </left>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dotted">
+        <color rgb="FF666666"/>
+      </left>
+      <right style="thin"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -468,7 +553,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -501,127 +586,163 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -702,15 +823,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="O28" activeCellId="0" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.0969387755102"/>
     <col collapsed="false" hidden="false" max="13" min="2" style="0" width="4.42857142857143"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="14.4285714285714"/>
   </cols>
@@ -873,13 +994,11 @@
       <c r="K10" s="9"/>
       <c r="L10" s="10"/>
       <c r="M10" s="12"/>
-      <c r="Q10" s="13" t="s">
-        <v>8</v>
-      </c>
+      <c r="Q10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
@@ -896,7 +1015,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
@@ -913,7 +1032,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
@@ -930,7 +1049,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
@@ -961,25 +1080,25 @@
       <c r="M15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26" t="n">
-        <v>2</v>
-      </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="30"/>
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="29"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="n">
-        <v>2</v>
+      <c r="A17" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
@@ -995,8 +1114,8 @@
       <c r="M17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="n">
-        <v>2</v>
+      <c r="A18" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -1012,21 +1131,21 @@
       <c r="M18" s="12"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="n">
-        <v>2</v>
-      </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="34"/>
+      <c r="A19" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="33"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19"/>
@@ -1043,26 +1162,26 @@
       <c r="L20" s="23"/>
       <c r="M20" s="24"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26" t="n">
-        <v>5</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="30"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="n">
-        <v>5</v>
+    <row r="21" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="29"/>
+    </row>
+    <row r="22" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="35" t="s">
+        <v>17</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
@@ -1077,9 +1196,9 @@
       <c r="L22" s="10"/>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="n">
-        <v>5</v>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="35" t="s">
+        <v>18</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
@@ -1094,22 +1213,22 @@
       <c r="L23" s="10"/>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="n">
-        <v>5</v>
-      </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="34"/>
+    <row r="24" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="33"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="20"/>
@@ -1127,25 +1246,25 @@
       <c r="M25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="26" t="n">
-        <v>10</v>
-      </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="30"/>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="n">
-        <v>10</v>
+      <c r="A26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="29"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="37" t="s">
+        <v>21</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
@@ -1160,9 +1279,9 @@
       <c r="L27" s="10"/>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="n">
-        <v>10</v>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="37" t="s">
+        <v>22</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
@@ -1177,25 +1296,25 @@
       <c r="L28" s="10"/>
       <c r="M28" s="12"/>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="n">
-        <v>10</v>
-      </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="34"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="33"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="35"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="25"/>
       <c r="C30" s="23"/>
       <c r="D30" s="24"/>
@@ -1209,112 +1328,63 @@
       <c r="L30" s="23"/>
       <c r="M30" s="24"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="30"/>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="12"/>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="12"/>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="34"/>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="41"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="44"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="45"/>
+      <c r="I33" s="45"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="47"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1322,9 +1392,9 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="A37:I37"/>
-    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A35:K35"/>
   </mergeCells>
   <conditionalFormatting sqref="B2">
     <cfRule type="colorScale" priority="2">

</xml_diff>